<commit_message>
jdt and start of message
</commit_message>
<xml_diff>
--- a/documents/JDT/JDT.xlsx
+++ b/documents/JDT/JDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\Mostly_Human\documents\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4779D9-4605-4838-85A9-D333E7ADF61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA227B35-052E-4A75-B477-C0F8EB9591A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E0F9514E-71B1-4D3A-A758-AA454C20BFD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E0F9514E-71B1-4D3A-A758-AA454C20BFD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Semaine1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="103">
   <si>
     <t xml:space="preserve">Semaine </t>
   </si>
@@ -336,6 +336,21 @@
   </si>
   <si>
     <t>ajout des logs sur la page avec la liste des pc actuellement scannés</t>
+  </si>
+  <si>
+    <t>Ajout de l'option pour supprimer une ressource de la liste principale de ressources bannies</t>
+  </si>
+  <si>
+    <t>sprint review 2</t>
+  </si>
+  <si>
+    <t>liason basique gRPC entre les 2 posts dans l'environement de dev</t>
+  </si>
+  <si>
+    <t>recherche</t>
+  </si>
+  <si>
+    <t>recherches sur les notifications window</t>
   </si>
 </sst>
 </file>
@@ -8216,10 +8231,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907C45BA-4F9F-41C5-A434-F4A1CDF997CE}">
-  <dimension ref="B2:M92"/>
+  <dimension ref="B2:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73:I74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8341,7 +8356,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="51">
-        <f>SUM(L19,L28,L45,L60,L91)</f>
+        <f>SUM(L19,L28,L45,L60,L77)</f>
         <v>0.90625</v>
       </c>
       <c r="C10" s="48"/>
@@ -9386,285 +9401,47 @@
       <c r="M76" s="50"/>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B77" s="39"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="44"/>
-      <c r="G77" s="44"/>
-      <c r="H77" s="44"/>
-      <c r="I77" s="40"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="40"/>
-      <c r="L77" s="47">
-        <v>0</v>
-      </c>
-      <c r="M77" s="48"/>
+      <c r="B77" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="63"/>
+      <c r="D77" s="63"/>
+      <c r="E77" s="63"/>
+      <c r="F77" s="63"/>
+      <c r="G77" s="63"/>
+      <c r="H77" s="63"/>
+      <c r="I77" s="63"/>
+      <c r="J77" s="63"/>
+      <c r="K77" s="63"/>
+      <c r="L77" s="70">
+        <f>SUM(L67:M76)</f>
+        <v>0.28125</v>
+      </c>
+      <c r="M77" s="71"/>
     </row>
     <row r="78" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="41"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="46"/>
-      <c r="F78" s="46"/>
-      <c r="G78" s="46"/>
-      <c r="H78" s="46"/>
-      <c r="I78" s="42"/>
-      <c r="J78" s="45"/>
-      <c r="K78" s="42"/>
-      <c r="L78" s="49"/>
-      <c r="M78" s="50"/>
-    </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B79" s="39"/>
-      <c r="C79" s="40"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="44"/>
-      <c r="H79" s="44"/>
-      <c r="I79" s="40"/>
-      <c r="J79" s="43"/>
-      <c r="K79" s="40"/>
-      <c r="L79" s="47">
-        <v>0</v>
-      </c>
-      <c r="M79" s="48"/>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B80" s="41"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="46"/>
-      <c r="H80" s="46"/>
-      <c r="I80" s="42"/>
-      <c r="J80" s="45"/>
-      <c r="K80" s="42"/>
-      <c r="L80" s="49"/>
-      <c r="M80" s="50"/>
-    </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B81" s="39"/>
-      <c r="C81" s="40"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="44"/>
-      <c r="F81" s="44"/>
-      <c r="G81" s="44"/>
-      <c r="H81" s="44"/>
-      <c r="I81" s="40"/>
-      <c r="J81" s="43"/>
-      <c r="K81" s="40"/>
-      <c r="L81" s="47">
-        <v>0</v>
-      </c>
-      <c r="M81" s="48"/>
-    </row>
-    <row r="82" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="41"/>
-      <c r="C82" s="42"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="46"/>
-      <c r="H82" s="46"/>
-      <c r="I82" s="42"/>
-      <c r="J82" s="45"/>
-      <c r="K82" s="42"/>
-      <c r="L82" s="49"/>
-      <c r="M82" s="50"/>
-    </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B83" s="39"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="44"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="43"/>
-      <c r="K83" s="40"/>
-      <c r="L83" s="47">
-        <v>0</v>
-      </c>
-      <c r="M83" s="48"/>
-    </row>
-    <row r="84" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="41"/>
-      <c r="C84" s="42"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="46"/>
-      <c r="F84" s="46"/>
-      <c r="G84" s="46"/>
-      <c r="H84" s="46"/>
-      <c r="I84" s="42"/>
-      <c r="J84" s="45"/>
-      <c r="K84" s="42"/>
-      <c r="L84" s="49"/>
-      <c r="M84" s="50"/>
-    </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B85" s="39"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="44"/>
-      <c r="F85" s="44"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="44"/>
-      <c r="I85" s="40"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="40"/>
-      <c r="L85" s="47">
-        <v>0</v>
-      </c>
-      <c r="M85" s="48"/>
-    </row>
-    <row r="86" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="41"/>
-      <c r="C86" s="42"/>
-      <c r="D86" s="45"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-      <c r="G86" s="46"/>
-      <c r="H86" s="46"/>
-      <c r="I86" s="42"/>
-      <c r="J86" s="45"/>
-      <c r="K86" s="42"/>
-      <c r="L86" s="49"/>
-      <c r="M86" s="50"/>
-    </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B87" s="66"/>
-      <c r="C87" s="54"/>
-      <c r="D87" s="68"/>
-      <c r="E87" s="54"/>
-      <c r="F87" s="54"/>
-      <c r="G87" s="54"/>
-      <c r="H87" s="54"/>
-      <c r="I87" s="54"/>
-      <c r="J87" s="68"/>
-      <c r="K87" s="54"/>
-      <c r="L87" s="47">
-        <v>0</v>
-      </c>
-      <c r="M87" s="48"/>
-    </row>
-    <row r="88" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="67"/>
-      <c r="C88" s="55"/>
-      <c r="D88" s="55"/>
-      <c r="E88" s="55"/>
-      <c r="F88" s="55"/>
-      <c r="G88" s="55"/>
-      <c r="H88" s="55"/>
-      <c r="I88" s="55"/>
-      <c r="J88" s="55"/>
-      <c r="K88" s="55"/>
-      <c r="L88" s="49"/>
-      <c r="M88" s="50"/>
-    </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B89" s="66"/>
-      <c r="C89" s="54"/>
-      <c r="D89" s="68"/>
-      <c r="E89" s="54"/>
-      <c r="F89" s="54"/>
-      <c r="G89" s="54"/>
-      <c r="H89" s="54"/>
-      <c r="I89" s="54"/>
-      <c r="J89" s="68"/>
-      <c r="K89" s="54"/>
-      <c r="L89" s="47">
-        <v>0</v>
-      </c>
-      <c r="M89" s="48"/>
-    </row>
-    <row r="90" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="67"/>
-      <c r="C90" s="55"/>
-      <c r="D90" s="55"/>
-      <c r="E90" s="55"/>
-      <c r="F90" s="55"/>
-      <c r="G90" s="55"/>
-      <c r="H90" s="55"/>
-      <c r="I90" s="55"/>
-      <c r="J90" s="55"/>
-      <c r="K90" s="55"/>
-      <c r="L90" s="49"/>
-      <c r="M90" s="50"/>
-    </row>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B91" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" s="63"/>
-      <c r="D91" s="63"/>
-      <c r="E91" s="63"/>
-      <c r="F91" s="63"/>
-      <c r="G91" s="63"/>
-      <c r="H91" s="63"/>
-      <c r="I91" s="63"/>
-      <c r="J91" s="63"/>
-      <c r="K91" s="63"/>
-      <c r="L91" s="70">
-        <f>SUM(L67:M90)</f>
-        <v>0.28125</v>
-      </c>
-      <c r="M91" s="71"/>
-    </row>
-    <row r="92" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="64"/>
-      <c r="C92" s="65"/>
-      <c r="D92" s="65"/>
-      <c r="E92" s="65"/>
-      <c r="F92" s="65"/>
-      <c r="G92" s="65"/>
-      <c r="H92" s="65"/>
-      <c r="I92" s="65"/>
-      <c r="J92" s="65"/>
-      <c r="K92" s="65"/>
-      <c r="L92" s="65"/>
-      <c r="M92" s="72"/>
+      <c r="B78" s="64"/>
+      <c r="C78" s="65"/>
+      <c r="D78" s="65"/>
+      <c r="E78" s="65"/>
+      <c r="F78" s="65"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="65"/>
+      <c r="J78" s="65"/>
+      <c r="K78" s="65"/>
+      <c r="L78" s="65"/>
+      <c r="M78" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="155">
-    <mergeCell ref="B91:C92"/>
-    <mergeCell ref="D91:K92"/>
-    <mergeCell ref="L91:M92"/>
-    <mergeCell ref="B87:C88"/>
-    <mergeCell ref="D87:I88"/>
-    <mergeCell ref="J87:K88"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="B89:C90"/>
-    <mergeCell ref="D89:I90"/>
-    <mergeCell ref="J89:K90"/>
-    <mergeCell ref="L89:M90"/>
-    <mergeCell ref="B83:C84"/>
-    <mergeCell ref="D83:I84"/>
-    <mergeCell ref="J83:K84"/>
-    <mergeCell ref="L83:M84"/>
-    <mergeCell ref="B85:C86"/>
-    <mergeCell ref="D85:I86"/>
-    <mergeCell ref="J85:K86"/>
-    <mergeCell ref="L85:M86"/>
-    <mergeCell ref="B79:C80"/>
-    <mergeCell ref="D79:I80"/>
-    <mergeCell ref="J79:K80"/>
-    <mergeCell ref="L79:M80"/>
-    <mergeCell ref="B81:C82"/>
-    <mergeCell ref="D81:I82"/>
-    <mergeCell ref="J81:K82"/>
-    <mergeCell ref="L81:M82"/>
+  <mergeCells count="127">
+    <mergeCell ref="B77:C78"/>
+    <mergeCell ref="D77:K78"/>
+    <mergeCell ref="L77:M78"/>
     <mergeCell ref="B75:C76"/>
     <mergeCell ref="D75:I76"/>
     <mergeCell ref="J75:K76"/>
     <mergeCell ref="L75:M76"/>
-    <mergeCell ref="B77:C78"/>
-    <mergeCell ref="D77:I78"/>
-    <mergeCell ref="J77:K78"/>
-    <mergeCell ref="L77:M78"/>
     <mergeCell ref="B71:C72"/>
     <mergeCell ref="D71:I72"/>
     <mergeCell ref="J71:K72"/>
@@ -9794,8 +9571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6889286-55A1-4118-911B-77969CD083C9}">
   <dimension ref="B2:M144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:I34"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9918,7 +9695,7 @@
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="51">
         <f>SUM(L41,L50,L81,L112,L143)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>0.21875</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="53">
@@ -9931,7 +9708,7 @@
       <c r="I10" s="54"/>
       <c r="J10" s="53">
         <f>D10-B10</f>
-        <v>0.88541666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="K10" s="54"/>
       <c r="L10" s="47">
@@ -10022,9 +9799,13 @@
       <c r="M16" s="11"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
+      <c r="B17" s="39" t="s">
+        <v>55</v>
+      </c>
       <c r="C17" s="40"/>
-      <c r="D17" s="43"/>
+      <c r="D17" s="43" t="s">
+        <v>98</v>
+      </c>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
@@ -10033,7 +9814,7 @@
       <c r="J17" s="43"/>
       <c r="K17" s="40"/>
       <c r="L17" s="47">
-        <v>2.0833333333333332E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="M17" s="48"/>
     </row>
@@ -10052,9 +9833,13 @@
       <c r="M18" s="50"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
+      <c r="B19" s="39" t="s">
+        <v>64</v>
+      </c>
       <c r="C19" s="40"/>
-      <c r="D19" s="43"/>
+      <c r="D19" s="43" t="s">
+        <v>99</v>
+      </c>
       <c r="E19" s="44"/>
       <c r="F19" s="44"/>
       <c r="G19" s="44"/>
@@ -10063,7 +9848,7 @@
       <c r="J19" s="43"/>
       <c r="K19" s="40"/>
       <c r="L19" s="47">
-        <v>0</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="M19" s="48"/>
     </row>
@@ -10082,9 +9867,13 @@
       <c r="M20" s="50"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
+      <c r="B21" s="39" t="s">
+        <v>55</v>
+      </c>
       <c r="C21" s="40"/>
-      <c r="D21" s="43"/>
+      <c r="D21" s="43" t="s">
+        <v>100</v>
+      </c>
       <c r="E21" s="44"/>
       <c r="F21" s="44"/>
       <c r="G21" s="44"/>
@@ -10093,7 +9882,7 @@
       <c r="J21" s="43"/>
       <c r="K21" s="40"/>
       <c r="L21" s="47">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M21" s="48"/>
     </row>
@@ -10112,9 +9901,13 @@
       <c r="M22" s="50"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="39"/>
+      <c r="B23" s="39" t="s">
+        <v>101</v>
+      </c>
       <c r="C23" s="40"/>
-      <c r="D23" s="43"/>
+      <c r="D23" s="43" t="s">
+        <v>54</v>
+      </c>
       <c r="E23" s="44"/>
       <c r="F23" s="44"/>
       <c r="G23" s="44"/>
@@ -10123,7 +9916,7 @@
       <c r="J23" s="43"/>
       <c r="K23" s="40"/>
       <c r="L23" s="47">
-        <v>0</v>
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="M23" s="48"/>
     </row>
@@ -10142,9 +9935,13 @@
       <c r="M24" s="50"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
+      <c r="B25" s="39" t="s">
+        <v>101</v>
+      </c>
       <c r="C25" s="40"/>
-      <c r="D25" s="43"/>
+      <c r="D25" s="43" t="s">
+        <v>102</v>
+      </c>
       <c r="E25" s="44"/>
       <c r="F25" s="44"/>
       <c r="G25" s="44"/>
@@ -10153,7 +9950,7 @@
       <c r="J25" s="43"/>
       <c r="K25" s="40"/>
       <c r="L25" s="47">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="M25" s="48"/>
     </row>
@@ -10396,7 +10193,7 @@
       <c r="K41" s="63"/>
       <c r="L41" s="70">
         <f>SUM(L17:M40)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>0.21875</v>
       </c>
       <c r="M41" s="71"/>
     </row>

</xml_diff>

<commit_message>
comment, documentation and jdt
</commit_message>
<xml_diff>
--- a/documents/JDT/JDT.xlsx
+++ b/documents/JDT/JDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\Mostly_Human\documents\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34A17F7-C44B-4F0B-A5BB-133E917C0AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF5C003-D3A3-48E6-A719-29C4814288AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E0F9514E-71B1-4D3A-A758-AA454C20BFD4}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="111">
   <si>
     <t xml:space="preserve">Semaine </t>
   </si>
@@ -360,6 +360,21 @@
   </si>
   <si>
     <t>recherches sur le multi threading</t>
+  </si>
+  <si>
+    <t>code/recherches</t>
+  </si>
+  <si>
+    <t>j'ai eu un problème avec grpc et la version de .NET, j'ai actuellement .Net 4.8 et il me faut la version 8 ou 9 mais j'arrive pas à l'installer dans vscode</t>
+  </si>
+  <si>
+    <t>optimisation de petites choses</t>
+  </si>
+  <si>
+    <t>ajout de commentaires ou il manquait, pas fini</t>
+  </si>
+  <si>
+    <t>avance sur la documentation</t>
   </si>
 </sst>
 </file>
@@ -8242,7 +8257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{907C45BA-4F9F-41C5-A434-F4A1CDF997CE}">
   <dimension ref="B2:M78"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:M36"/>
     </sheetView>
   </sheetViews>
@@ -9580,8 +9595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6889286-55A1-4118-911B-77969CD083C9}">
   <dimension ref="B2:M130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51:M52"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="O76" sqref="O76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9704,7 +9719,7 @@
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="51">
         <f>SUM(L27,L36,L67,L98,L129)</f>
-        <v>0.43055555555555558</v>
+        <v>0.625</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="53">
@@ -9717,7 +9732,7 @@
       <c r="I10" s="54"/>
       <c r="J10" s="53">
         <f>D10-B10</f>
-        <v>0.47569444444444442</v>
+        <v>0.28125</v>
       </c>
       <c r="K10" s="54"/>
       <c r="L10" s="47">
@@ -10259,7 +10274,7 @@
       <c r="J45" s="43"/>
       <c r="K45" s="40"/>
       <c r="L45" s="47">
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M45" s="48"/>
     </row>
@@ -10293,7 +10308,7 @@
       <c r="J47" s="43"/>
       <c r="K47" s="40"/>
       <c r="L47" s="47">
-        <v>0.125</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="M47" s="48"/>
     </row>
@@ -10327,7 +10342,7 @@
       <c r="J49" s="43"/>
       <c r="K49" s="40"/>
       <c r="L49" s="47">
-        <v>6.25E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="M49" s="48"/>
     </row>
@@ -10346,9 +10361,13 @@
       <c r="M50" s="50"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="39"/>
+      <c r="B51" s="39" t="s">
+        <v>55</v>
+      </c>
       <c r="C51" s="40"/>
-      <c r="D51" s="43"/>
+      <c r="D51" s="43" t="s">
+        <v>108</v>
+      </c>
       <c r="E51" s="44"/>
       <c r="F51" s="44"/>
       <c r="G51" s="44"/>
@@ -10357,7 +10376,7 @@
       <c r="J51" s="43"/>
       <c r="K51" s="40"/>
       <c r="L51" s="47">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="M51" s="48"/>
     </row>
@@ -10600,7 +10619,7 @@
       <c r="K67" s="63"/>
       <c r="L67" s="70">
         <f>SUM(L43:M66)</f>
-        <v>0.21180555555555555</v>
+        <v>0.28125</v>
       </c>
       <c r="M67" s="71"/>
     </row>
@@ -10686,9 +10705,13 @@
       <c r="M73" s="11"/>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="39"/>
+      <c r="B74" s="39" t="s">
+        <v>64</v>
+      </c>
       <c r="C74" s="40"/>
-      <c r="D74" s="43"/>
+      <c r="D74" s="43" t="s">
+        <v>65</v>
+      </c>
       <c r="E74" s="44"/>
       <c r="F74" s="44"/>
       <c r="G74" s="44"/>
@@ -10697,7 +10720,7 @@
       <c r="J74" s="43"/>
       <c r="K74" s="40"/>
       <c r="L74" s="47">
-        <v>0</v>
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="M74" s="48"/>
     </row>
@@ -10715,10 +10738,14 @@
       <c r="L75" s="49"/>
       <c r="M75" s="50"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="39"/>
+    <row r="76" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="39" t="s">
+        <v>106</v>
+      </c>
       <c r="C76" s="40"/>
-      <c r="D76" s="43"/>
+      <c r="D76" s="43" t="s">
+        <v>107</v>
+      </c>
       <c r="E76" s="44"/>
       <c r="F76" s="44"/>
       <c r="G76" s="44"/>
@@ -10727,7 +10754,7 @@
       <c r="J76" s="43"/>
       <c r="K76" s="40"/>
       <c r="L76" s="47">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M76" s="48"/>
     </row>
@@ -10746,9 +10773,13 @@
       <c r="M77" s="50"/>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78" s="39"/>
+      <c r="B78" s="39" t="s">
+        <v>47</v>
+      </c>
       <c r="C78" s="40"/>
-      <c r="D78" s="43"/>
+      <c r="D78" s="43" t="s">
+        <v>110</v>
+      </c>
       <c r="E78" s="44"/>
       <c r="F78" s="44"/>
       <c r="G78" s="44"/>
@@ -10757,7 +10788,7 @@
       <c r="J78" s="43"/>
       <c r="K78" s="40"/>
       <c r="L78" s="47">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="M78" s="48"/>
     </row>
@@ -10776,9 +10807,13 @@
       <c r="M79" s="50"/>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B80" s="39"/>
+      <c r="B80" s="39" t="s">
+        <v>55</v>
+      </c>
       <c r="C80" s="40"/>
-      <c r="D80" s="43"/>
+      <c r="D80" s="43" t="s">
+        <v>109</v>
+      </c>
       <c r="E80" s="44"/>
       <c r="F80" s="44"/>
       <c r="G80" s="44"/>
@@ -10787,7 +10822,7 @@
       <c r="J80" s="43"/>
       <c r="K80" s="40"/>
       <c r="L80" s="47">
-        <v>0</v>
+        <v>3.8194444444444441E-2</v>
       </c>
       <c r="M80" s="48"/>
     </row>
@@ -11060,7 +11095,7 @@
       <c r="K98" s="63"/>
       <c r="L98" s="70">
         <f>SUM(L74:M97)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="M98" s="71"/>
     </row>

</xml_diff>

<commit_message>
update doc and jdt
</commit_message>
<xml_diff>
--- a/documents/JDT/JDT.xlsx
+++ b/documents/JDT/JDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg66hua\Documents\GitHub\Mostly_Human\documents\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F39196F-BC4E-4531-94F7-BBE40B2A058D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0450A1-6A17-4775-B5F8-01EB87734D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{E0F9514E-71B1-4D3A-A758-AA454C20BFD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{E0F9514E-71B1-4D3A-A758-AA454C20BFD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Semaine1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,8 @@
     <sheet name="Semaine3" sheetId="9" r:id="rId3"/>
     <sheet name="Semaine4" sheetId="10" r:id="rId4"/>
     <sheet name="Semaine5" sheetId="11" r:id="rId5"/>
-    <sheet name="Graphique1" sheetId="14" r:id="rId6"/>
-    <sheet name="Semaine6" sheetId="12" r:id="rId7"/>
-    <sheet name="Semaine7" sheetId="13" r:id="rId8"/>
+    <sheet name="Semaine6" sheetId="12" r:id="rId6"/>
+    <sheet name="Semaine7" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="128">
   <si>
     <t xml:space="preserve">Semaine </t>
   </si>
@@ -418,6 +417,15 @@
   </si>
   <si>
     <t>Implementation du heart beat (console à serveur) -&gt; prochaine étape, lancer le heart beat depuis la GUI</t>
+  </si>
+  <si>
+    <t>sprint review 3</t>
+  </si>
+  <si>
+    <t>problème avec des réferances en boucle (2 object qui ont une référence de l'autre -&gt; problème) [WIP]</t>
+  </si>
+  <si>
+    <t>Implementation du heart beat à la partie form [WIP]</t>
   </si>
 </sst>
 </file>
@@ -916,809 +924,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="373266704"/>
-        <c:axId val="373836528"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="373266704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="373836528"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="373836528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="373266704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79DA4814-3879-4558-815A-58D1DF11E348}">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30919177-788A-2F4D-22A2-9850FFB8E097}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -10441,7 +9646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6889286-55A1-4118-911B-77969CD083C9}">
   <dimension ref="B2:M86"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
@@ -11909,6 +11114,9 @@
     <mergeCell ref="D73:I74"/>
     <mergeCell ref="J73:K74"/>
     <mergeCell ref="L73:M74"/>
+    <mergeCell ref="B85:C86"/>
+    <mergeCell ref="D85:K86"/>
+    <mergeCell ref="L85:M86"/>
     <mergeCell ref="B83:C84"/>
     <mergeCell ref="D83:I84"/>
     <mergeCell ref="J83:K84"/>
@@ -11921,9 +11129,6 @@
     <mergeCell ref="D81:I82"/>
     <mergeCell ref="J81:K82"/>
     <mergeCell ref="L81:M82"/>
-    <mergeCell ref="B85:C86"/>
-    <mergeCell ref="D85:K86"/>
-    <mergeCell ref="L85:M86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11931,10 +11136,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47395D2-1B8B-46E3-90B4-08378D46F65A}">
-  <dimension ref="B2:M120"/>
+  <dimension ref="B2:M92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="N64" sqref="N64"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="N87" sqref="N87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12056,8 +11261,8 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="41">
-        <f>SUM(L29,L38,L57,L88,L119)</f>
-        <v>0.5625</v>
+        <f>SUM(L29,L38,L57,L72,L91)</f>
+        <v>0.84375</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="43">
@@ -12070,7 +11275,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="43">
         <f>D10-B10</f>
-        <v>0.34375</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="18">
@@ -13037,740 +12242,344 @@
       <c r="M71" s="21"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="22"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="26"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="23"/>
-      <c r="J72" s="26"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="18">
-        <v>0</v>
-      </c>
-      <c r="M72" s="19"/>
+      <c r="B72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="6">
+        <f>SUM(L64:M71)</f>
+        <v>0.125</v>
+      </c>
+      <c r="M72" s="7"/>
     </row>
     <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="24"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="29"/>
-      <c r="F73" s="29"/>
-      <c r="G73" s="29"/>
-      <c r="H73" s="29"/>
-      <c r="I73" s="25"/>
-      <c r="J73" s="28"/>
-      <c r="K73" s="25"/>
-      <c r="L73" s="20"/>
-      <c r="M73" s="21"/>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="22"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="26"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="27"/>
-      <c r="G74" s="27"/>
-      <c r="H74" s="27"/>
-      <c r="I74" s="23"/>
-      <c r="J74" s="26"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="18">
-        <v>0</v>
-      </c>
-      <c r="M74" s="19"/>
-    </row>
-    <row r="75" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="29"/>
-      <c r="F75" s="29"/>
-      <c r="G75" s="29"/>
-      <c r="H75" s="29"/>
-      <c r="I75" s="25"/>
-      <c r="J75" s="28"/>
-      <c r="K75" s="25"/>
-      <c r="L75" s="20"/>
-      <c r="M75" s="21"/>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="22"/>
-      <c r="C76" s="23"/>
-      <c r="D76" s="26"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="23"/>
-      <c r="J76" s="26"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="18">
-        <v>0</v>
-      </c>
-      <c r="M76" s="19"/>
-    </row>
-    <row r="77" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="24"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="29"/>
-      <c r="I77" s="25"/>
-      <c r="J77" s="28"/>
-      <c r="K77" s="25"/>
-      <c r="L77" s="20"/>
-      <c r="M77" s="21"/>
-    </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78" s="22"/>
-      <c r="C78" s="23"/>
-      <c r="D78" s="26"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="27"/>
-      <c r="H78" s="27"/>
-      <c r="I78" s="23"/>
-      <c r="J78" s="26"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="18">
-        <v>0</v>
-      </c>
-      <c r="M78" s="19"/>
-    </row>
-    <row r="79" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="24"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="28"/>
-      <c r="E79" s="29"/>
-      <c r="F79" s="29"/>
-      <c r="G79" s="29"/>
-      <c r="H79" s="29"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="28"/>
-      <c r="K79" s="25"/>
-      <c r="L79" s="20"/>
-      <c r="M79" s="21"/>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B80" s="22"/>
-      <c r="C80" s="23"/>
-      <c r="D80" s="26"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="23"/>
-      <c r="J80" s="26"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="18">
-        <v>0</v>
-      </c>
-      <c r="M80" s="19"/>
-    </row>
-    <row r="81" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="24"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
-      <c r="G81" s="29"/>
-      <c r="H81" s="29"/>
-      <c r="I81" s="25"/>
-      <c r="J81" s="28"/>
-      <c r="K81" s="25"/>
-      <c r="L81" s="20"/>
-      <c r="M81" s="21"/>
-    </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B82" s="22"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="26"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
-      <c r="I82" s="23"/>
-      <c r="J82" s="26"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="18">
-        <v>0</v>
-      </c>
-      <c r="M82" s="19"/>
-    </row>
-    <row r="83" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="24"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="29"/>
-      <c r="H83" s="29"/>
-      <c r="I83" s="25"/>
-      <c r="J83" s="28"/>
-      <c r="K83" s="25"/>
-      <c r="L83" s="20"/>
-      <c r="M83" s="21"/>
-    </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B84" s="22"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="26"/>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="27"/>
-      <c r="H84" s="27"/>
-      <c r="I84" s="23"/>
-      <c r="J84" s="26"/>
-      <c r="K84" s="23"/>
-      <c r="L84" s="18">
-        <v>0</v>
-      </c>
-      <c r="M84" s="19"/>
-    </row>
-    <row r="85" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="24"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="29"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="29"/>
-      <c r="I85" s="25"/>
-      <c r="J85" s="28"/>
-      <c r="K85" s="25"/>
-      <c r="L85" s="20"/>
-      <c r="M85" s="21"/>
-    </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B86" s="22"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="26"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="27"/>
-      <c r="H86" s="27"/>
-      <c r="I86" s="23"/>
-      <c r="J86" s="26"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="18">
-        <v>0</v>
-      </c>
-      <c r="M86" s="19"/>
-    </row>
-    <row r="87" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="24"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="29"/>
-      <c r="G87" s="29"/>
-      <c r="H87" s="29"/>
-      <c r="I87" s="25"/>
-      <c r="J87" s="28"/>
-      <c r="K87" s="25"/>
-      <c r="L87" s="20"/>
-      <c r="M87" s="21"/>
-    </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
+      <c r="B73" s="4"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="8"/>
+    </row>
+    <row r="74" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B75" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
+      <c r="I75" s="32"/>
+      <c r="J75" s="32"/>
+      <c r="K75" s="32"/>
+      <c r="L75" s="32"/>
+      <c r="M75" s="35"/>
+    </row>
+    <row r="76" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="33"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="34"/>
+      <c r="H76" s="34"/>
+      <c r="I76" s="34"/>
+      <c r="J76" s="34"/>
+      <c r="K76" s="34"/>
+      <c r="L76" s="34"/>
+      <c r="M76" s="36"/>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B77" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="37"/>
+      <c r="D77" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K77" s="37"/>
+      <c r="L77" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M77" s="37"/>
+    </row>
+    <row r="78" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="11"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="38"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="38"/>
+      <c r="L78" s="11"/>
+      <c r="M78" s="38"/>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B79" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" s="23"/>
+      <c r="D79" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E79" s="27"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="23"/>
+      <c r="J79" s="26"/>
+      <c r="K79" s="23"/>
+      <c r="L79" s="18">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="M79" s="19"/>
+    </row>
+    <row r="80" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="25"/>
+      <c r="J80" s="28"/>
+      <c r="K80" s="25"/>
+      <c r="L80" s="20"/>
+      <c r="M80" s="21"/>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B81" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" s="23"/>
+      <c r="D81" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="23"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="23"/>
+      <c r="L81" s="18">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M81" s="19"/>
+    </row>
+    <row r="82" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="24"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="25"/>
+      <c r="J82" s="28"/>
+      <c r="K82" s="25"/>
+      <c r="L82" s="20"/>
+      <c r="M82" s="21"/>
+    </row>
+    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B83" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="23"/>
+      <c r="D83" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="27"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="23"/>
+      <c r="L83" s="18">
+        <v>9.375E-2</v>
+      </c>
+      <c r="M83" s="19"/>
+    </row>
+    <row r="84" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="24"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="25"/>
+      <c r="J84" s="28"/>
+      <c r="K84" s="25"/>
+      <c r="L84" s="20"/>
+      <c r="M84" s="21"/>
+    </row>
+    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B85" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="23"/>
+      <c r="D85" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E85" s="27"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="27"/>
+      <c r="H85" s="27"/>
+      <c r="I85" s="23"/>
+      <c r="J85" s="26"/>
+      <c r="K85" s="23"/>
+      <c r="L85" s="18">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="M85" s="19"/>
+    </row>
+    <row r="86" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="24"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="25"/>
+      <c r="J86" s="28"/>
+      <c r="K86" s="25"/>
+      <c r="L86" s="20"/>
+      <c r="M86" s="21"/>
+    </row>
+    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B87" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" s="23"/>
+      <c r="D87" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="23"/>
+      <c r="J87" s="26"/>
+      <c r="K87" s="23"/>
+      <c r="L87" s="18">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="M87" s="19"/>
+    </row>
+    <row r="88" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="24"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="28"/>
+      <c r="K88" s="25"/>
+      <c r="L88" s="20"/>
+      <c r="M88" s="21"/>
+    </row>
+    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B89" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" s="23"/>
+      <c r="D89" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="27"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="26"/>
+      <c r="K89" s="23"/>
+      <c r="L89" s="18">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="M89" s="19"/>
+    </row>
+    <row r="90" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="24"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="25"/>
+      <c r="J90" s="28"/>
+      <c r="K90" s="25"/>
+      <c r="L90" s="20"/>
+      <c r="M90" s="21"/>
+    </row>
+    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-      <c r="L88" s="6">
-        <f>SUM(L64:M87)</f>
-        <v>0.125</v>
-      </c>
-      <c r="M88" s="7"/>
-    </row>
-    <row r="89" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="4"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-      <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
-      <c r="M89" s="8"/>
-    </row>
-    <row r="90" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B91" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C91" s="32"/>
-      <c r="D91" s="32"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="32"/>
-      <c r="H91" s="32"/>
-      <c r="I91" s="32"/>
-      <c r="J91" s="32"/>
-      <c r="K91" s="32"/>
-      <c r="L91" s="32"/>
-      <c r="M91" s="35"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="6">
+        <f>SUM(L79:M90)</f>
+        <v>0.28125</v>
+      </c>
+      <c r="M91" s="7"/>
     </row>
     <row r="92" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="33"/>
-      <c r="C92" s="34"/>
-      <c r="D92" s="34"/>
-      <c r="E92" s="34"/>
-      <c r="F92" s="34"/>
-      <c r="G92" s="34"/>
-      <c r="H92" s="34"/>
-      <c r="I92" s="34"/>
-      <c r="J92" s="34"/>
-      <c r="K92" s="34"/>
-      <c r="L92" s="34"/>
-      <c r="M92" s="36"/>
-    </row>
-    <row r="93" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B93" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="37"/>
-      <c r="D93" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E93" s="10"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
-      <c r="H93" s="10"/>
-      <c r="I93" s="37"/>
-      <c r="J93" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K93" s="37"/>
-      <c r="L93" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M93" s="37"/>
-    </row>
-    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B94" s="11"/>
-      <c r="C94" s="38"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="12"/>
-      <c r="I94" s="38"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="38"/>
-      <c r="L94" s="11"/>
-      <c r="M94" s="38"/>
-    </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B95" s="22"/>
-      <c r="C95" s="23"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="27"/>
-      <c r="I95" s="23"/>
-      <c r="J95" s="26"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="18">
-        <v>0</v>
-      </c>
-      <c r="M95" s="19"/>
-    </row>
-    <row r="96" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="24"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
-      <c r="G96" s="29"/>
-      <c r="H96" s="29"/>
-      <c r="I96" s="25"/>
-      <c r="J96" s="28"/>
-      <c r="K96" s="25"/>
-      <c r="L96" s="20"/>
-      <c r="M96" s="21"/>
-    </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B97" s="22"/>
-      <c r="C97" s="23"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="27"/>
-      <c r="I97" s="23"/>
-      <c r="J97" s="26"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="18">
-        <v>0</v>
-      </c>
-      <c r="M97" s="19"/>
-    </row>
-    <row r="98" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="24"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="29"/>
-      <c r="F98" s="29"/>
-      <c r="G98" s="29"/>
-      <c r="H98" s="29"/>
-      <c r="I98" s="25"/>
-      <c r="J98" s="28"/>
-      <c r="K98" s="25"/>
-      <c r="L98" s="20"/>
-      <c r="M98" s="21"/>
-    </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B99" s="22"/>
-      <c r="C99" s="23"/>
-      <c r="D99" s="26"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="23"/>
-      <c r="J99" s="26"/>
-      <c r="K99" s="23"/>
-      <c r="L99" s="18">
-        <v>0</v>
-      </c>
-      <c r="M99" s="19"/>
-    </row>
-    <row r="100" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="24"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="29"/>
-      <c r="F100" s="29"/>
-      <c r="G100" s="29"/>
-      <c r="H100" s="29"/>
-      <c r="I100" s="25"/>
-      <c r="J100" s="28"/>
-      <c r="K100" s="25"/>
-      <c r="L100" s="20"/>
-      <c r="M100" s="21"/>
-    </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B101" s="22"/>
-      <c r="C101" s="23"/>
-      <c r="D101" s="26"/>
-      <c r="E101" s="27"/>
-      <c r="F101" s="27"/>
-      <c r="G101" s="27"/>
-      <c r="H101" s="27"/>
-      <c r="I101" s="23"/>
-      <c r="J101" s="26"/>
-      <c r="K101" s="23"/>
-      <c r="L101" s="18">
-        <v>0</v>
-      </c>
-      <c r="M101" s="19"/>
-    </row>
-    <row r="102" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="24"/>
-      <c r="C102" s="25"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="29"/>
-      <c r="F102" s="29"/>
-      <c r="G102" s="29"/>
-      <c r="H102" s="29"/>
-      <c r="I102" s="25"/>
-      <c r="J102" s="28"/>
-      <c r="K102" s="25"/>
-      <c r="L102" s="20"/>
-      <c r="M102" s="21"/>
-    </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B103" s="22"/>
-      <c r="C103" s="23"/>
-      <c r="D103" s="26"/>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="27"/>
-      <c r="H103" s="27"/>
-      <c r="I103" s="23"/>
-      <c r="J103" s="26"/>
-      <c r="K103" s="23"/>
-      <c r="L103" s="18">
-        <v>0</v>
-      </c>
-      <c r="M103" s="19"/>
-    </row>
-    <row r="104" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="24"/>
-      <c r="C104" s="25"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="29"/>
-      <c r="G104" s="29"/>
-      <c r="H104" s="29"/>
-      <c r="I104" s="25"/>
-      <c r="J104" s="28"/>
-      <c r="K104" s="25"/>
-      <c r="L104" s="20"/>
-      <c r="M104" s="21"/>
-    </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B105" s="22"/>
-      <c r="C105" s="23"/>
-      <c r="D105" s="26"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
-      <c r="G105" s="27"/>
-      <c r="H105" s="27"/>
-      <c r="I105" s="23"/>
-      <c r="J105" s="26"/>
-      <c r="K105" s="23"/>
-      <c r="L105" s="18">
-        <v>0</v>
-      </c>
-      <c r="M105" s="19"/>
-    </row>
-    <row r="106" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="24"/>
-      <c r="C106" s="25"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="29"/>
-      <c r="F106" s="29"/>
-      <c r="G106" s="29"/>
-      <c r="H106" s="29"/>
-      <c r="I106" s="25"/>
-      <c r="J106" s="28"/>
-      <c r="K106" s="25"/>
-      <c r="L106" s="20"/>
-      <c r="M106" s="21"/>
-    </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B107" s="22"/>
-      <c r="C107" s="23"/>
-      <c r="D107" s="26"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
-      <c r="I107" s="23"/>
-      <c r="J107" s="26"/>
-      <c r="K107" s="23"/>
-      <c r="L107" s="18">
-        <v>0</v>
-      </c>
-      <c r="M107" s="19"/>
-    </row>
-    <row r="108" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="24"/>
-      <c r="C108" s="25"/>
-      <c r="D108" s="28"/>
-      <c r="E108" s="29"/>
-      <c r="F108" s="29"/>
-      <c r="G108" s="29"/>
-      <c r="H108" s="29"/>
-      <c r="I108" s="25"/>
-      <c r="J108" s="28"/>
-      <c r="K108" s="25"/>
-      <c r="L108" s="20"/>
-      <c r="M108" s="21"/>
-    </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B109" s="22"/>
-      <c r="C109" s="23"/>
-      <c r="D109" s="26"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="23"/>
-      <c r="J109" s="26"/>
-      <c r="K109" s="23"/>
-      <c r="L109" s="18">
-        <v>0</v>
-      </c>
-      <c r="M109" s="19"/>
-    </row>
-    <row r="110" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="24"/>
-      <c r="C110" s="25"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="29"/>
-      <c r="F110" s="29"/>
-      <c r="G110" s="29"/>
-      <c r="H110" s="29"/>
-      <c r="I110" s="25"/>
-      <c r="J110" s="28"/>
-      <c r="K110" s="25"/>
-      <c r="L110" s="20"/>
-      <c r="M110" s="21"/>
-    </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B111" s="22"/>
-      <c r="C111" s="23"/>
-      <c r="D111" s="26"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="27"/>
-      <c r="H111" s="27"/>
-      <c r="I111" s="23"/>
-      <c r="J111" s="26"/>
-      <c r="K111" s="23"/>
-      <c r="L111" s="18">
-        <v>0</v>
-      </c>
-      <c r="M111" s="19"/>
-    </row>
-    <row r="112" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="24"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="29"/>
-      <c r="F112" s="29"/>
-      <c r="G112" s="29"/>
-      <c r="H112" s="29"/>
-      <c r="I112" s="25"/>
-      <c r="J112" s="28"/>
-      <c r="K112" s="25"/>
-      <c r="L112" s="20"/>
-      <c r="M112" s="21"/>
-    </row>
-    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B113" s="22"/>
-      <c r="C113" s="23"/>
-      <c r="D113" s="26"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="27"/>
-      <c r="G113" s="27"/>
-      <c r="H113" s="27"/>
-      <c r="I113" s="23"/>
-      <c r="J113" s="26"/>
-      <c r="K113" s="23"/>
-      <c r="L113" s="18">
-        <v>0</v>
-      </c>
-      <c r="M113" s="19"/>
-    </row>
-    <row r="114" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="24"/>
-      <c r="C114" s="25"/>
-      <c r="D114" s="28"/>
-      <c r="E114" s="29"/>
-      <c r="F114" s="29"/>
-      <c r="G114" s="29"/>
-      <c r="H114" s="29"/>
-      <c r="I114" s="25"/>
-      <c r="J114" s="28"/>
-      <c r="K114" s="25"/>
-      <c r="L114" s="20"/>
-      <c r="M114" s="21"/>
-    </row>
-    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B115" s="13"/>
-      <c r="C115" s="14"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="14"/>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
-      <c r="J115" s="17"/>
-      <c r="K115" s="14"/>
-      <c r="L115" s="18">
-        <v>0</v>
-      </c>
-      <c r="M115" s="19"/>
-    </row>
-    <row r="116" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="15"/>
-      <c r="C116" s="16"/>
-      <c r="D116" s="16"/>
-      <c r="E116" s="16"/>
-      <c r="F116" s="16"/>
-      <c r="G116" s="16"/>
-      <c r="H116" s="16"/>
-      <c r="I116" s="16"/>
-      <c r="J116" s="16"/>
-      <c r="K116" s="16"/>
-      <c r="L116" s="20"/>
-      <c r="M116" s="21"/>
-    </row>
-    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B117" s="13"/>
-      <c r="C117" s="14"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
-      <c r="G117" s="14"/>
-      <c r="H117" s="14"/>
-      <c r="I117" s="14"/>
-      <c r="J117" s="17"/>
-      <c r="K117" s="14"/>
-      <c r="L117" s="18">
-        <v>0</v>
-      </c>
-      <c r="M117" s="19"/>
-    </row>
-    <row r="118" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="15"/>
-      <c r="C118" s="16"/>
-      <c r="D118" s="16"/>
-      <c r="E118" s="16"/>
-      <c r="F118" s="16"/>
-      <c r="G118" s="16"/>
-      <c r="H118" s="16"/>
-      <c r="I118" s="16"/>
-      <c r="J118" s="16"/>
-      <c r="K118" s="16"/>
-      <c r="L118" s="20"/>
-      <c r="M118" s="21"/>
-    </row>
-    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B119" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="H119" s="3"/>
-      <c r="I119" s="3"/>
-      <c r="J119" s="3"/>
-      <c r="K119" s="3"/>
-      <c r="L119" s="6">
-        <f>SUM(L95:M118)</f>
-        <v>0</v>
-      </c>
-      <c r="M119" s="7"/>
-    </row>
-    <row r="120" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="4"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="5"/>
-      <c r="I120" s="5"/>
-      <c r="J120" s="5"/>
-      <c r="K120" s="5"/>
-      <c r="L120" s="5"/>
-      <c r="M120" s="8"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="5"/>
+      <c r="L92" s="5"/>
+      <c r="M92" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="211">
+  <mergeCells count="155">
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="D10:I11"/>
     <mergeCell ref="J10:K11"/>
@@ -13890,98 +12699,42 @@
     <mergeCell ref="D66:I67"/>
     <mergeCell ref="J66:K67"/>
     <mergeCell ref="L66:M67"/>
-    <mergeCell ref="B76:C77"/>
-    <mergeCell ref="D76:I77"/>
-    <mergeCell ref="J76:K77"/>
-    <mergeCell ref="L76:M77"/>
-    <mergeCell ref="B78:C79"/>
-    <mergeCell ref="D78:I79"/>
-    <mergeCell ref="J78:K79"/>
-    <mergeCell ref="L78:M79"/>
+    <mergeCell ref="B79:C80"/>
+    <mergeCell ref="D79:I80"/>
+    <mergeCell ref="J79:K80"/>
+    <mergeCell ref="L79:M80"/>
+    <mergeCell ref="B83:C84"/>
+    <mergeCell ref="D83:I84"/>
+    <mergeCell ref="J81:K82"/>
+    <mergeCell ref="L81:M82"/>
     <mergeCell ref="B72:C73"/>
-    <mergeCell ref="D72:I73"/>
-    <mergeCell ref="J72:K73"/>
+    <mergeCell ref="D72:K73"/>
     <mergeCell ref="L72:M73"/>
-    <mergeCell ref="B74:C75"/>
-    <mergeCell ref="D74:I75"/>
-    <mergeCell ref="J74:K75"/>
-    <mergeCell ref="L74:M75"/>
-    <mergeCell ref="B84:C85"/>
-    <mergeCell ref="D84:I85"/>
-    <mergeCell ref="J84:K85"/>
-    <mergeCell ref="L84:M85"/>
-    <mergeCell ref="B86:C87"/>
-    <mergeCell ref="D86:I87"/>
-    <mergeCell ref="J86:K87"/>
-    <mergeCell ref="L86:M87"/>
-    <mergeCell ref="B80:C81"/>
-    <mergeCell ref="D80:I81"/>
-    <mergeCell ref="J80:K81"/>
-    <mergeCell ref="L80:M81"/>
-    <mergeCell ref="B82:C83"/>
-    <mergeCell ref="D82:I83"/>
-    <mergeCell ref="J82:K83"/>
-    <mergeCell ref="L82:M83"/>
-    <mergeCell ref="B95:C96"/>
-    <mergeCell ref="D95:I96"/>
-    <mergeCell ref="J95:K96"/>
-    <mergeCell ref="L95:M96"/>
-    <mergeCell ref="B97:C98"/>
-    <mergeCell ref="D97:I98"/>
-    <mergeCell ref="J97:K98"/>
-    <mergeCell ref="L97:M98"/>
-    <mergeCell ref="B88:C89"/>
-    <mergeCell ref="D88:K89"/>
-    <mergeCell ref="L88:M89"/>
-    <mergeCell ref="B91:K92"/>
+    <mergeCell ref="B75:K76"/>
+    <mergeCell ref="L75:M76"/>
+    <mergeCell ref="B77:C78"/>
+    <mergeCell ref="D77:I78"/>
+    <mergeCell ref="J77:K78"/>
+    <mergeCell ref="L77:M78"/>
+    <mergeCell ref="B81:C82"/>
+    <mergeCell ref="D81:I82"/>
+    <mergeCell ref="J87:K88"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="B89:C90"/>
+    <mergeCell ref="D89:I90"/>
+    <mergeCell ref="J89:K90"/>
+    <mergeCell ref="L89:M90"/>
+    <mergeCell ref="B85:C86"/>
+    <mergeCell ref="D85:I86"/>
+    <mergeCell ref="J83:K84"/>
+    <mergeCell ref="L83:M84"/>
+    <mergeCell ref="B87:C88"/>
+    <mergeCell ref="D87:I88"/>
+    <mergeCell ref="J85:K86"/>
+    <mergeCell ref="L85:M86"/>
+    <mergeCell ref="B91:C92"/>
+    <mergeCell ref="D91:K92"/>
     <mergeCell ref="L91:M92"/>
-    <mergeCell ref="B93:C94"/>
-    <mergeCell ref="D93:I94"/>
-    <mergeCell ref="J93:K94"/>
-    <mergeCell ref="L93:M94"/>
-    <mergeCell ref="B103:C104"/>
-    <mergeCell ref="D103:I104"/>
-    <mergeCell ref="J103:K104"/>
-    <mergeCell ref="L103:M104"/>
-    <mergeCell ref="B105:C106"/>
-    <mergeCell ref="D105:I106"/>
-    <mergeCell ref="J105:K106"/>
-    <mergeCell ref="L105:M106"/>
-    <mergeCell ref="B99:C100"/>
-    <mergeCell ref="D99:I100"/>
-    <mergeCell ref="J99:K100"/>
-    <mergeCell ref="L99:M100"/>
-    <mergeCell ref="B101:C102"/>
-    <mergeCell ref="D101:I102"/>
-    <mergeCell ref="J101:K102"/>
-    <mergeCell ref="L101:M102"/>
-    <mergeCell ref="B111:C112"/>
-    <mergeCell ref="D111:I112"/>
-    <mergeCell ref="J111:K112"/>
-    <mergeCell ref="L111:M112"/>
-    <mergeCell ref="B113:C114"/>
-    <mergeCell ref="D113:I114"/>
-    <mergeCell ref="J113:K114"/>
-    <mergeCell ref="L113:M114"/>
-    <mergeCell ref="B107:C108"/>
-    <mergeCell ref="D107:I108"/>
-    <mergeCell ref="J107:K108"/>
-    <mergeCell ref="L107:M108"/>
-    <mergeCell ref="B109:C110"/>
-    <mergeCell ref="D109:I110"/>
-    <mergeCell ref="J109:K110"/>
-    <mergeCell ref="L109:M110"/>
-    <mergeCell ref="B119:C120"/>
-    <mergeCell ref="D119:K120"/>
-    <mergeCell ref="L119:M120"/>
-    <mergeCell ref="B115:C116"/>
-    <mergeCell ref="D115:I116"/>
-    <mergeCell ref="J115:K116"/>
-    <mergeCell ref="L115:M116"/>
-    <mergeCell ref="B117:C118"/>
-    <mergeCell ref="D117:I118"/>
-    <mergeCell ref="J117:K118"/>
-    <mergeCell ref="L117:M118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>